<commit_message>
update all the files
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VII.xlsx
+++ b/inc/flattened/createYaml/VII.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/Desktop/Current-Projects/ParserTools/createYaml/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A66638-BF57-C54B-884C-33CBAE80B6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BF3DF4-E1B4-1F45-9AD7-BA1A84FF357A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
   </bookViews>
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:I257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11450,6 +11450,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDA4FEBE11D32545B6C4D443ADFB229A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa29c2c3225ad03fb09b8df90fa91a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b103a3be-6c61-44b0-93c5-2b779aa38a01" xmlns:ns3="56612388-9f28-4625-93a0-6879c02082d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c16c82533632c11d7fcceef7f9e9ea5" ns2:_="" ns3:_="">
     <xsd:import namespace="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
@@ -11614,15 +11623,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
   <ds:schemaRefs>
@@ -11641,6 +11641,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CADB2AF-8FF4-4CD3-86AB-7AA08F493F37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11657,12 +11665,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>